<commit_message>
added Dove Springs location and simplified maps a bit
</commit_message>
<xml_diff>
--- a/Austin_Public_Health_Locations.xlsx
+++ b/Austin_Public_Health_Locations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5260" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Austin_Public_Health_Locations " sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="203">
   <si>
     <t>Facility Name</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>Other Location</t>
+  </si>
+  <si>
+    <t>Dove Springs Neighborhood Public Health Facility</t>
+  </si>
+  <si>
+    <t>5106 Village Square Drive, Austin, Texas 78744</t>
   </si>
 </sst>
 </file>
@@ -1003,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2492,6 +2498,26 @@
         <v>-97.637159999999994</v>
       </c>
     </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>201</v>
+      </c>
+      <c r="B32" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" t="s">
+        <v>202</v>
+      </c>
+      <c r="D32">
+        <v>78744</v>
+      </c>
+      <c r="E32">
+        <v>30.188171000000001</v>
+      </c>
+      <c r="F32">
+        <v>-97.744249999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>